<commit_message>
completed backend for admin
</commit_message>
<xml_diff>
--- a/report_data/22CS168/report.xlsx
+++ b/report_data/22CS168/report.xlsx
@@ -14,27 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>15.5.23</t>
-  </si>
-  <si>
-    <t>16.5.23</t>
-  </si>
-  <si>
-    <t>17.5.23</t>
-  </si>
-  <si>
-    <t>18.5.23</t>
-  </si>
-  <si>
-    <t>19.5.23</t>
-  </si>
-  <si>
-    <t>20.5.23</t>
+    <t>11.9.23</t>
+  </si>
+  <si>
+    <t>12.9.23</t>
+  </si>
+  <si>
+    <t>13.9.23</t>
+  </si>
+  <si>
+    <t>14.9.23</t>
+  </si>
+  <si>
+    <t>15.9.23</t>
+  </si>
+  <si>
+    <t>16.9.23</t>
   </si>
   <si>
     <t>Total No</t>
@@ -52,148 +52,172 @@
     <t>MON</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>18.9.2023</t>
+  </si>
+  <si>
+    <t>25.9.2023</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>22.5.23</t>
-  </si>
-  <si>
-    <t>29.5.23</t>
-  </si>
-  <si>
-    <t>5.6.23</t>
-  </si>
-  <si>
-    <t>12.6.23</t>
+    <t>2.10.2023</t>
+  </si>
+  <si>
+    <t>9.10.2023</t>
+  </si>
+  <si>
+    <t>16.10.2023</t>
   </si>
   <si>
     <t>TUE</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>23.5.23</t>
-  </si>
-  <si>
-    <t>30.5.23</t>
-  </si>
-  <si>
-    <t>6.6.23</t>
-  </si>
-  <si>
-    <t>13.6.23</t>
+    <t>19.9.2023</t>
+  </si>
+  <si>
+    <t>26.9.2023</t>
+  </si>
+  <si>
+    <t>3.10.2023</t>
+  </si>
+  <si>
+    <t>10.10.2023</t>
+  </si>
+  <si>
+    <t>17.10.2023</t>
   </si>
   <si>
     <t>WED</t>
   </si>
   <si>
-    <t>24.5.23</t>
-  </si>
-  <si>
-    <t>31.5.23</t>
-  </si>
-  <si>
-    <t>7.6.23</t>
-  </si>
-  <si>
-    <t>14.6.23</t>
+    <t>20.9.2023</t>
+  </si>
+  <si>
+    <t>27.9.2023</t>
+  </si>
+  <si>
+    <t>4.10.2023</t>
+  </si>
+  <si>
+    <t>11.10.2023</t>
+  </si>
+  <si>
+    <t>18.10.2023</t>
   </si>
   <si>
     <t>THU</t>
   </si>
   <si>
-    <t>25.5.23</t>
-  </si>
-  <si>
-    <t>1.6.23</t>
-  </si>
-  <si>
-    <t>8.6.23</t>
-  </si>
-  <si>
-    <t>15.6.23</t>
+    <t>21.9.2023</t>
+  </si>
+  <si>
+    <t>28.9.2023</t>
+  </si>
+  <si>
+    <t>5.10.2023</t>
+  </si>
+  <si>
+    <t>12.10.2023</t>
+  </si>
+  <si>
+    <t>19.10.2023</t>
   </si>
   <si>
     <t>FRI</t>
   </si>
   <si>
-    <t>26.5.23</t>
-  </si>
-  <si>
-    <t>2.6.23</t>
-  </si>
-  <si>
-    <t>9.6.23</t>
-  </si>
-  <si>
-    <t>16.6.23</t>
+    <t>22.9.2023</t>
+  </si>
+  <si>
+    <t>29.9.2023</t>
+  </si>
+  <si>
+    <t>6.10.2023</t>
+  </si>
+  <si>
+    <t>13.10.2023</t>
+  </si>
+  <si>
+    <t>20.10.2023</t>
   </si>
   <si>
     <t>SAT</t>
   </si>
   <si>
-    <t>27.5.23</t>
-  </si>
-  <si>
-    <t>3.6.23</t>
-  </si>
-  <si>
-    <t>10.6.23</t>
-  </si>
-  <si>
-    <t>17.6.23</t>
+    <t>23.9.2023</t>
+  </si>
+  <si>
+    <t>30.9.2023</t>
+  </si>
+  <si>
+    <t>7.10.2023</t>
+  </si>
+  <si>
+    <t>14.10.2023</t>
+  </si>
+  <si>
+    <t>21.10.2023</t>
   </si>
   <si>
     <t>of Hours</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>180</t>
+    <t>28</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>164</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>219</t>
+    <t>70</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>202</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>51.28205128205128</t>
-  </si>
-  <si>
-    <t>75.5813953488372</t>
-  </si>
-  <si>
-    <t>78.19548872180451</t>
-  </si>
-  <si>
-    <t>81.97674418604652</t>
-  </si>
-  <si>
-    <t>82.1917808219178</t>
+    <t>71.7948717948718</t>
+  </si>
+  <si>
+    <t>72.85714285714285</t>
+  </si>
+  <si>
+    <t>74.19354838709677</t>
+  </si>
+  <si>
+    <t>78.52760736196319</t>
+  </si>
+  <si>
+    <t>81.1881188118812</t>
   </si>
 </sst>
 </file>
@@ -551,31 +575,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:AR18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="9" width="3.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
     <col min="19" max="24" width="3.7109375" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
     <col min="26" max="32" width="3.7109375" customWidth="1"/>
-    <col min="33" max="33" width="7.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
     <col min="34" max="40" width="3.7109375" customWidth="1"/>
-    <col min="41" max="41" width="7.7109375" customWidth="1"/>
-    <col min="42" max="48" width="3.7109375" customWidth="1"/>
-    <col min="49" max="49" width="8.7109375" customWidth="1"/>
-    <col min="50" max="50" width="10.7109375" customWidth="1"/>
-    <col min="51" max="51" width="17.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" customWidth="1"/>
+    <col min="42" max="42" width="8.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,38 +722,17 @@
       <c r="AO1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AP1" s="1">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>42</v>
+      <c r="AP1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="AR1" s="1">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="1">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="1">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY1" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -738,31 +740,31 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AO2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW2" t="s">
         <v>43</v>
       </c>
-      <c r="AX2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>54</v>
+      <c r="AP2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:44">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -770,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -791,43 +793,43 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>1</v>
@@ -836,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -860,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="AG3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AH3">
         <v>1</v>
@@ -875,25 +877,25 @@
         <v>1</v>
       </c>
       <c r="AL3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN3">
-        <v>1</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:44">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -901,110 +903,86 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Y4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AG4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AO4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AW4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP4" t="s">
         <v>7</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AQ4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:44">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AO5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW5" t="s">
         <v>43</v>
       </c>
-      <c r="AX5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>54</v>
+      <c r="AP5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:44">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1025,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="Y6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z6">
         <v>1</v>
@@ -1049,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="AG6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AH6">
         <v>1</v>
@@ -1072,41 +1050,17 @@
       <c r="AN6">
         <v>1</v>
       </c>
-      <c r="AO6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-      <c r="AR6">
-        <v>1</v>
-      </c>
-      <c r="AS6">
-        <v>1</v>
-      </c>
-      <c r="AT6">
-        <v>1</v>
-      </c>
-      <c r="AU6">
-        <v>1</v>
-      </c>
-      <c r="AV6">
-        <v>1</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>56</v>
+      <c r="AP6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:44">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1114,28 +1068,28 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Y7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AG7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AO7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP7" t="s">
         <v>7</v>
       </c>
-      <c r="AX7" t="s">
+      <c r="AQ7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:44">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1143,36 +1097,36 @@
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AO8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW8" t="s">
         <v>43</v>
       </c>
-      <c r="AX8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>54</v>
+      <c r="AP8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:44">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1196,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1220,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -1235,123 +1189,51 @@
         <v>1</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <v>1</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-      <c r="AC9">
-        <v>1</v>
-      </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
-      <c r="AE9">
-        <v>1</v>
-      </c>
-      <c r="AF9">
-        <v>1</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH9">
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <v>1</v>
-      </c>
-      <c r="AJ9">
-        <v>1</v>
-      </c>
-      <c r="AK9">
-        <v>1</v>
-      </c>
-      <c r="AL9">
-        <v>1</v>
-      </c>
-      <c r="AM9">
-        <v>1</v>
-      </c>
-      <c r="AN9">
-        <v>1</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP9">
-        <v>1</v>
-      </c>
-      <c r="AQ9">
-        <v>0</v>
-      </c>
-      <c r="AR9">
-        <v>0</v>
-      </c>
-      <c r="AS9">
-        <v>0</v>
-      </c>
-      <c r="AT9">
-        <v>1</v>
-      </c>
-      <c r="AU9">
-        <v>1</v>
-      </c>
-      <c r="AV9">
-        <v>1</v>
-      </c>
-      <c r="AW9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO10" t="s">
         <v>46</v>
       </c>
-      <c r="AX9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>57</v>
+      <c r="AP10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="R10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:44">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1359,84 +1241,60 @@
         <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AO11" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW11" t="s">
         <v>43</v>
       </c>
-      <c r="AX11" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>54</v>
+      <c r="AP11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:44">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="J12" t="s">
         <v>12</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S12">
         <v>1</v>
@@ -1451,13 +1309,13 @@
         <v>1</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z12">
         <v>1</v>
@@ -1481,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="AG12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AH12">
         <v>1</v>
@@ -1504,46 +1362,46 @@
       <c r="AN12">
         <v>1</v>
       </c>
-      <c r="AW12" t="s">
+      <c r="AP12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO13" t="s">
         <v>47</v>
       </c>
-      <c r="AX12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>58</v>
+      <c r="AP13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:51">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:44">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1551,36 +1409,36 @@
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AG14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AO14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW14" t="s">
         <v>43</v>
       </c>
-      <c r="AX14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY14" t="s">
-        <v>54</v>
+      <c r="AP14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:44">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1604,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1619,16 +1477,16 @@
         <v>1</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S15">
         <v>1</v>
@@ -1643,13 +1501,13 @@
         <v>1</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z15">
         <v>1</v>
@@ -1673,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="AG15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AH15">
         <v>1</v>
@@ -1688,46 +1546,214 @@
         <v>1</v>
       </c>
       <c r="AL15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN15">
-        <v>0</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP15">
-        <v>1</v>
-      </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
-      <c r="AR15">
-        <v>0</v>
-      </c>
-      <c r="AS15">
-        <v>0</v>
-      </c>
-      <c r="AT15">
-        <v>1</v>
-      </c>
-      <c r="AU15">
-        <v>1</v>
-      </c>
-      <c r="AV15">
-        <v>1</v>
-      </c>
-      <c r="AW15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO16" t="s">
         <v>48</v>
       </c>
-      <c r="AX15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY15" t="s">
-        <v>59</v>
+      <c r="AP16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>